<commit_message>
pt_upload based on country program
</commit_message>
<xml_diff>
--- a/data/kin_section4_narratives.xlsx
+++ b/data/kin_section4_narratives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rythomas\Documents\R_scripts\country_scorecards\country_scorecards\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C36D8E3-2B65-40B9-BB8F-176E3091D186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FFD2A3-3FAB-4968-B751-E3EFC3186C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{08F4287E-D4FA-4E4B-9BD0-8619EF0B0FA0}"/>
   </bookViews>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C91B05F-CBCD-4F47-9DF8-6A19E569FD6C}">
   <dimension ref="A1:D252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:XFD91"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>